<commit_message>
Types doorgevoerd in hpm en ich en excel bestanden
</commit_message>
<xml_diff>
--- a/src/main/resources/nhs-dmn/OriginelenVoorBusiness/icf_Interpretatie_CF_Origineel.xlsx
+++ b/src/main/resources/nhs-dmn/OriginelenVoorBusiness/icf_Interpretatie_CF_Origineel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\han\git\rivm\nhs\dmn\nhs-business\src\main\resources\nhs-dmn\OriginelenVoorBusiness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DE4DA2-D8C0-4A11-8C04-1D9490A1D67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588E8D83-B87C-4299-B785-8D2A6F92FDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36750" yWindow="-765" windowWidth="21600" windowHeight="11295" tabRatio="834" activeTab="3" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
+    <workbookView xWindow="31395" yWindow="480" windowWidth="21600" windowHeight="11295" tabRatio="834" activeTab="1" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
   </bookViews>
   <sheets>
     <sheet name="Lijstjes" sheetId="7" r:id="rId1"/>
@@ -189,28 +189,28 @@
     <t>InterpretatieEGABlad1</t>
   </si>
   <si>
-    <t>HPM.waarde("IRT")</t>
-  </si>
-  <si>
-    <t>HPM.waarde("PAP")</t>
-  </si>
-  <si>
-    <t>HPM.waarde("DNA_N")</t>
-  </si>
-  <si>
-    <t>HPM.waarde("DNA_imut1")</t>
-  </si>
-  <si>
-    <t>HPM.waarde("DNA_imut2")</t>
-  </si>
-  <si>
-    <t>HPM.waarde("EGA_N")</t>
-  </si>
-  <si>
-    <t>HPM.waarde("EGA_imut1")</t>
-  </si>
-  <si>
-    <t>HPM.waarde("EGA_imut2")</t>
+    <t>HPM.waardeNum("EGA_N")</t>
+  </si>
+  <si>
+    <t>HPM.waardeString("EGA_imut1")</t>
+  </si>
+  <si>
+    <t>HPM.waardeString("EGA_imut2")</t>
+  </si>
+  <si>
+    <t>HPM.waardeString("DNA_imut1")</t>
+  </si>
+  <si>
+    <t>HPM.waardeString("DNA_imut2")</t>
+  </si>
+  <si>
+    <t>HPM.waardeNum("DNA_N")</t>
+  </si>
+  <si>
+    <t>HPM.waardeNum("PAP")</t>
+  </si>
+  <si>
+    <t>HPM.waardeNum("IRT")</t>
   </si>
 </sst>
 </file>
@@ -384,10 +384,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -941,29 +937,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE86461-8803-4D16-98CE-5EF23E3CB8A1}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>45</v>
@@ -1890,25 +1886,23 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>41</v>
@@ -2290,23 +2284,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB09FB6-758D-4B28-8B58-73E92576AEB6}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>40</v>

</xml_diff>